<commit_message>
Resnet excel graph now in GB
</commit_message>
<xml_diff>
--- a/final_report/thesis_charts.xlsx
+++ b/final_report/thesis_charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izaak\Document\engsci_thesis\final_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1D6647-8B57-42F9-B99E-10500401B3C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1981A9AA-574D-4EB7-A028-15201EE390E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41280" yWindow="9075" windowWidth="19635" windowHeight="15435" activeTab="1" xr2:uid="{5D6391EE-4981-4592-A0FD-F1E471CC3565}"/>
   </bookViews>
@@ -923,11 +923,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -996,10 +1003,12 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1071,7 +1080,9 @@
               <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1387,7 +1398,7 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Memory (MB)</a:t>
+                  <a:t>Memory (GB)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1455,6 +1466,9 @@
         <c:crossAx val="520240448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3089,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CF0BFC-766E-4E95-8FDD-8AFE6159604F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>